<commit_message>
adding indexes, first merge, merging all in all, missingness analysis
</commit_message>
<xml_diff>
--- a/EMV_Data.xlsx
+++ b/EMV_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kyle Kost\Dropbox\RA_Perl_files\results_scraping\Excel Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\smribei\Desktop\UFMG-20180924T133728Z-001\Mestrado\Artigo\Analise de Sentimento\TimeSeriesArticle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3560BD2-D605-476B-8484-CBF98370FB05}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BB4DF9B-BB38-45C6-A5F3-A1945861C9F3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EMV Index" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>Year</t>
   </si>
@@ -168,9 +168,6 @@
     <t>Agricultural Policy EMV Tracker</t>
   </si>
   <si>
-    <t>Source: “Policy News and Stock Market Volatility” by Scott Baker, Nicholas Bloom, Steven J. Davis and Kyle Kost, 2019. These data can be used freely with attribution to the authors, the paper, and www.PolicyUncertainty.com.</t>
-  </si>
-  <si>
     <t>Infectious Disease EMV Tracker</t>
   </si>
 </sst>
@@ -265,7 +262,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -587,19 +584,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AT427"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView tabSelected="1" topLeftCell="A401" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A427" sqref="A427"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="8.5703125" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" customWidth="1"/>
-    <col min="4" max="5" width="8.85546875" customWidth="1"/>
-    <col min="6" max="1026" width="8.5703125" customWidth="1"/>
+    <col min="1" max="2" width="8.5546875" customWidth="1"/>
+    <col min="3" max="3" width="13.88671875" customWidth="1"/>
+    <col min="4" max="5" width="8.88671875" customWidth="1"/>
+    <col min="6" max="1026" width="8.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -613,7 +610,7 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
@@ -739,7 +736,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1985</v>
       </c>
@@ -879,7 +876,7 @@
         <v>8.0742979049682612E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1985</v>
       </c>
@@ -1019,7 +1016,7 @@
         <v>8.0869560567741722E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1985</v>
       </c>
@@ -1159,7 +1156,7 @@
         <v>8.2688991288493441E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1985</v>
       </c>
@@ -1299,7 +1296,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1985</v>
       </c>
@@ -1439,7 +1436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1985</v>
       </c>
@@ -1579,7 +1576,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1985</v>
       </c>
@@ -1719,7 +1716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1985</v>
       </c>
@@ -1859,7 +1856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1985</v>
       </c>
@@ -1999,7 +1996,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1985</v>
       </c>
@@ -2139,7 +2136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>1985</v>
       </c>
@@ -2279,7 +2276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>1985</v>
       </c>
@@ -2419,7 +2416,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>1986</v>
       </c>
@@ -2559,7 +2556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>1986</v>
       </c>
@@ -2699,7 +2696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>1986</v>
       </c>
@@ -2839,7 +2836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>1986</v>
       </c>
@@ -2979,7 +2976,7 @@
         <v>6.5257299514043896E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>1986</v>
       </c>
@@ -3119,7 +3116,7 @@
         <v>6.942118038921237E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>1986</v>
       </c>
@@ -3259,7 +3256,7 @@
         <v>6.0891686063824287E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>1986</v>
       </c>
@@ -3399,7 +3396,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>1986</v>
       </c>
@@ -3539,7 +3536,7 @@
         <v>0.13574217740820829</v>
       </c>
     </row>
-    <row r="22" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>1986</v>
       </c>
@@ -3679,7 +3676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>1986</v>
       </c>
@@ -3819,7 +3816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>1986</v>
       </c>
@@ -3959,7 +3956,7 @@
         <v>6.2608585098749919E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>1986</v>
       </c>
@@ -4099,7 +4096,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>1987</v>
       </c>
@@ -4239,7 +4236,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>1987</v>
       </c>
@@ -4379,7 +4376,7 @@
         <v>5.8843304412533541E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>1987</v>
       </c>
@@ -4519,7 +4516,7 @@
         <v>0.10534097867853501</v>
       </c>
     </row>
-    <row r="29" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>1987</v>
       </c>
@@ -4659,7 +4656,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>1987</v>
       </c>
@@ -4799,7 +4796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>1987</v>
       </c>
@@ -4939,7 +4936,7 @@
         <v>0.1655664638597138</v>
       </c>
     </row>
-    <row r="32" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>1987</v>
       </c>
@@ -5079,7 +5076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>1987</v>
       </c>
@@ -5219,7 +5216,7 @@
         <v>5.2191019058227539E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>1987</v>
       </c>
@@ -5359,7 +5356,7 @@
         <v>0.14695297511277999</v>
       </c>
     </row>
-    <row r="35" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>1987</v>
       </c>
@@ -5499,7 +5496,7 @@
         <v>0.10977599400631129</v>
       </c>
     </row>
-    <row r="36" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>1987</v>
       </c>
@@ -5639,7 +5636,7 @@
         <v>0.16886717765057674</v>
       </c>
     </row>
-    <row r="37" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>1987</v>
       </c>
@@ -5779,7 +5776,7 @@
         <v>5.4540708467557833E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>1988</v>
       </c>
@@ -5919,7 +5916,7 @@
         <v>5.4831264058097462E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>1988</v>
       </c>
@@ -6059,7 +6056,7 @@
         <v>0.16547058262956252</v>
       </c>
     </row>
-    <row r="40" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>1988</v>
       </c>
@@ -6199,7 +6196,7 @@
         <v>0.10089583780573702</v>
       </c>
     </row>
-    <row r="41" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>1988</v>
       </c>
@@ -6339,7 +6336,7 @@
         <v>0.11028905698873927</v>
       </c>
     </row>
-    <row r="42" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>1988</v>
       </c>
@@ -6479,7 +6476,7 @@
         <v>0.11034998686417288</v>
       </c>
     </row>
-    <row r="43" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>1988</v>
       </c>
@@ -6619,7 +6616,7 @@
         <v>0.20269248485565186</v>
       </c>
     </row>
-    <row r="44" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>1988</v>
       </c>
@@ -6759,7 +6756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>1988</v>
       </c>
@@ -6899,7 +6896,7 @@
         <v>5.3956846396128334E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>1988</v>
       </c>
@@ -7039,7 +7036,7 @@
         <v>0.10065926205028188</v>
       </c>
     </row>
-    <row r="47" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>1988</v>
       </c>
@@ -7179,7 +7176,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>1988</v>
       </c>
@@ -7319,7 +7316,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>1988</v>
       </c>
@@ -7459,7 +7456,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>1989</v>
       </c>
@@ -7599,7 +7596,7 @@
         <v>5.4671217492744749E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>1989</v>
       </c>
@@ -7739,7 +7736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>1989</v>
       </c>
@@ -7879,7 +7876,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>1989</v>
       </c>
@@ -8019,7 +8016,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>1989</v>
       </c>
@@ -8159,7 +8156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>1989</v>
       </c>
@@ -8299,7 +8296,7 @@
         <v>9.9993895131645472E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>1989</v>
       </c>
@@ -8439,7 +8436,7 @@
         <v>0.15624806730454149</v>
       </c>
     </row>
-    <row r="57" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>1989</v>
       </c>
@@ -8579,7 +8576,7 @@
         <v>5.2755436842045728E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>1989</v>
       </c>
@@ -8719,7 +8716,7 @@
         <v>0.1468450625737508</v>
       </c>
     </row>
-    <row r="59" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>1989</v>
       </c>
@@ -8859,7 +8856,7 @@
         <v>4.7385847631363956E-2</v>
       </c>
     </row>
-    <row r="60" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>1989</v>
       </c>
@@ -8999,7 +8996,7 @@
         <v>5.0209901419030617E-2</v>
       </c>
     </row>
-    <row r="61" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>1989</v>
       </c>
@@ -9139,7 +9136,7 @@
         <v>0.20101016400808314</v>
       </c>
     </row>
-    <row r="62" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>1990</v>
       </c>
@@ -9279,7 +9276,7 @@
         <v>4.8216118002837559E-2</v>
       </c>
     </row>
-    <row r="63" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>1990</v>
       </c>
@@ -9419,7 +9416,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>1990</v>
       </c>
@@ -9559,7 +9556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>1990</v>
       </c>
@@ -9699,7 +9696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>1990</v>
       </c>
@@ -9839,7 +9836,7 @@
         <v>4.2014085584216647E-2</v>
       </c>
     </row>
-    <row r="67" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>1990</v>
       </c>
@@ -9979,7 +9976,7 @@
         <v>4.901764514672495E-2</v>
       </c>
     </row>
-    <row r="68" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>1990</v>
       </c>
@@ -10119,7 +10116,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>1990</v>
       </c>
@@ -10259,7 +10256,7 @@
         <v>9.5220896008710837E-2</v>
       </c>
     </row>
-    <row r="70" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>1990</v>
       </c>
@@ -10399,7 +10396,7 @@
         <v>0.15137593043332842</v>
       </c>
     </row>
-    <row r="71" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>1990</v>
       </c>
@@ -10539,7 +10536,7 @@
         <v>5.1405181511690094E-2</v>
       </c>
     </row>
-    <row r="72" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>1990</v>
       </c>
@@ -10679,7 +10676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>1990</v>
       </c>
@@ -10819,7 +10816,7 @@
         <v>0.21545765187480662</v>
       </c>
     </row>
-    <row r="74" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>1991</v>
       </c>
@@ -10959,7 +10956,7 @@
         <v>0.10418583280477092</v>
       </c>
     </row>
-    <row r="75" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>1991</v>
       </c>
@@ -11099,7 +11096,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>1991</v>
       </c>
@@ -11239,7 +11236,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>1991</v>
       </c>
@@ -11379,7 +11376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>1991</v>
       </c>
@@ -11519,7 +11516,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>1991</v>
       </c>
@@ -11659,7 +11656,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>1991</v>
       </c>
@@ -11799,7 +11796,7 @@
         <v>5.7129536034925932E-2</v>
       </c>
     </row>
-    <row r="81" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>1991</v>
       </c>
@@ -11939,7 +11936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>1991</v>
       </c>
@@ -12079,7 +12076,7 @@
         <v>0.10543832778930665</v>
       </c>
     </row>
-    <row r="83" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>1991</v>
       </c>
@@ -12219,7 +12216,7 @@
         <v>5.1513911160555752E-2</v>
       </c>
     </row>
-    <row r="84" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>1991</v>
       </c>
@@ -12359,7 +12356,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>1991</v>
       </c>
@@ -12499,7 +12496,7 @@
         <v>0.10188700314674769</v>
       </c>
     </row>
-    <row r="86" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>1992</v>
       </c>
@@ -12639,7 +12636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>1992</v>
       </c>
@@ -12779,7 +12776,7 @@
         <v>5.6507356288069382E-2</v>
       </c>
     </row>
-    <row r="88" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>1992</v>
       </c>
@@ -12919,7 +12916,7 @@
         <v>5.1118174300026208E-2</v>
       </c>
     </row>
-    <row r="89" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>1992</v>
       </c>
@@ -13059,7 +13056,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>1992</v>
       </c>
@@ -13199,7 +13196,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>1992</v>
       </c>
@@ -13339,7 +13336,7 @@
         <v>0.16371536940979445</v>
       </c>
     </row>
-    <row r="92" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>1992</v>
       </c>
@@ -13479,7 +13476,7 @@
         <v>9.9120663924955985E-2</v>
       </c>
     </row>
-    <row r="93" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>1992</v>
       </c>
@@ -13619,7 +13616,7 @@
         <v>8.7831956626725022E-2</v>
       </c>
     </row>
-    <row r="94" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>1992</v>
       </c>
@@ -13759,7 +13756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>1992</v>
       </c>
@@ -13899,7 +13896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>1992</v>
       </c>
@@ -14039,7 +14036,7 @@
         <v>4.8167697667288699E-2</v>
       </c>
     </row>
-    <row r="97" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>1992</v>
       </c>
@@ -14179,7 +14176,7 @@
         <v>4.8577083770885217E-2</v>
       </c>
     </row>
-    <row r="98" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>1993</v>
       </c>
@@ -14319,7 +14316,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>1993</v>
       </c>
@@ -14459,7 +14456,7 @@
         <v>0.11923481101420388</v>
       </c>
     </row>
-    <row r="100" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>1993</v>
       </c>
@@ -14599,7 +14596,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>1993</v>
       </c>
@@ -14739,7 +14736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>1993</v>
       </c>
@@ -14879,7 +14876,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>1993</v>
       </c>
@@ -15019,7 +15016,7 @@
         <v>5.6575327429152625E-2</v>
       </c>
     </row>
-    <row r="104" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>1993</v>
       </c>
@@ -15159,7 +15156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>1993</v>
       </c>
@@ -15299,7 +15296,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>1993</v>
       </c>
@@ -15439,7 +15436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>1993</v>
       </c>
@@ -15579,7 +15576,7 @@
         <v>5.1500481250239351E-2</v>
       </c>
     </row>
-    <row r="108" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>1993</v>
       </c>
@@ -15719,7 +15716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>1993</v>
       </c>
@@ -15859,7 +15856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>1994</v>
       </c>
@@ -15999,7 +15996,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>1994</v>
       </c>
@@ -16139,7 +16136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>1994</v>
       </c>
@@ -16279,7 +16276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>1994</v>
       </c>
@@ -16419,7 +16416,7 @@
         <v>5.7406477646441634E-2</v>
       </c>
     </row>
-    <row r="114" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>1994</v>
       </c>
@@ -16559,7 +16556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>1994</v>
       </c>
@@ -16699,7 +16696,7 @@
         <v>0.14785337933039261</v>
       </c>
     </row>
-    <row r="116" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>1994</v>
       </c>
@@ -16839,7 +16836,7 @@
         <v>5.7132179428726337E-2</v>
       </c>
     </row>
-    <row r="117" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>1994</v>
       </c>
@@ -16979,7 +16976,7 @@
         <v>0.10208284144864933</v>
       </c>
     </row>
-    <row r="118" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>1994</v>
       </c>
@@ -17119,7 +17116,7 @@
         <v>5.6286257526934794E-2</v>
       </c>
     </row>
-    <row r="119" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>1994</v>
       </c>
@@ -17259,7 +17256,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>1994</v>
       </c>
@@ -17399,7 +17396,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>1994</v>
       </c>
@@ -17539,7 +17536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>1995</v>
       </c>
@@ -17679,7 +17676,7 @@
         <v>0.10884454617133509</v>
       </c>
     </row>
-    <row r="123" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>1995</v>
       </c>
@@ -17819,7 +17816,7 @@
         <v>6.2813143663003418E-2</v>
       </c>
     </row>
-    <row r="124" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>1995</v>
       </c>
@@ -17959,7 +17956,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>1995</v>
       </c>
@@ -18099,7 +18096,7 @@
         <v>0.1082023711741581</v>
       </c>
     </row>
-    <row r="126" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>1995</v>
       </c>
@@ -18239,7 +18236,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>1995</v>
       </c>
@@ -18379,7 +18376,7 @@
         <v>5.7775356672786694E-2</v>
       </c>
     </row>
-    <row r="128" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>1995</v>
       </c>
@@ -18519,7 +18516,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>1995</v>
       </c>
@@ -18659,7 +18656,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>1995</v>
       </c>
@@ -18799,7 +18796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>1995</v>
       </c>
@@ -18939,7 +18936,7 @@
         <v>5.4818183947832153E-2</v>
       </c>
     </row>
-    <row r="132" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>1995</v>
       </c>
@@ -19079,7 +19076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>1995</v>
       </c>
@@ -19219,7 +19216,7 @@
         <v>6.0610041522339682E-2</v>
       </c>
     </row>
-    <row r="134" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>1996</v>
       </c>
@@ -19359,7 +19356,7 @@
         <v>0.19874694439353152</v>
       </c>
     </row>
-    <row r="135" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>1996</v>
       </c>
@@ -19499,7 +19496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>1996</v>
       </c>
@@ -19639,7 +19636,7 @@
         <v>5.8142984793083059E-2</v>
       </c>
     </row>
-    <row r="137" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>1996</v>
       </c>
@@ -19779,7 +19776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>1996</v>
       </c>
@@ -19919,7 +19916,7 @@
         <v>0.1113477470048892</v>
       </c>
     </row>
-    <row r="139" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>1996</v>
       </c>
@@ -20059,7 +20056,7 @@
         <v>5.9877762188740587E-2</v>
       </c>
     </row>
-    <row r="140" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>1996</v>
       </c>
@@ -20199,7 +20196,7 @@
         <v>6.2474766162910852E-2</v>
       </c>
     </row>
-    <row r="141" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>1996</v>
       </c>
@@ -20339,7 +20336,7 @@
         <v>6.2589261069226618E-2</v>
       </c>
     </row>
-    <row r="142" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>1996</v>
       </c>
@@ -20479,7 +20476,7 @@
         <v>0.11086857318878174</v>
       </c>
     </row>
-    <row r="143" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>1996</v>
       </c>
@@ -20619,7 +20616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>1996</v>
       </c>
@@ -20759,7 +20756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>1996</v>
       </c>
@@ -20899,7 +20896,7 @@
         <v>5.9377057985825973E-2</v>
       </c>
     </row>
-    <row r="146" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>1997</v>
       </c>
@@ -21039,7 +21036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>1997</v>
       </c>
@@ -21179,7 +21176,7 @@
         <v>5.4876144839004735E-2</v>
       </c>
     </row>
-    <row r="148" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A148">
         <v>1997</v>
       </c>
@@ -21319,7 +21316,7 @@
         <v>0.10530358060784296</v>
       </c>
     </row>
-    <row r="149" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A149">
         <v>1997</v>
       </c>
@@ -21459,7 +21456,7 @@
         <v>0.1109866829805596</v>
       </c>
     </row>
-    <row r="150" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A150">
         <v>1997</v>
       </c>
@@ -21599,7 +21596,7 @@
         <v>5.2410086113904283E-2</v>
       </c>
     </row>
-    <row r="151" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A151">
         <v>1997</v>
       </c>
@@ -21739,7 +21736,7 @@
         <v>0.15773642970825816</v>
       </c>
     </row>
-    <row r="152" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A152">
         <v>1997</v>
       </c>
@@ -21879,7 +21876,7 @@
         <v>0.23056433541434151</v>
       </c>
     </row>
-    <row r="153" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A153">
         <v>1997</v>
       </c>
@@ -22019,7 +22016,7 @@
         <v>0.105010986328125</v>
       </c>
     </row>
-    <row r="154" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A154">
         <v>1997</v>
       </c>
@@ -22159,7 +22156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A155">
         <v>1997</v>
       </c>
@@ -22299,7 +22296,7 @@
         <v>5.0157225205123057E-2</v>
       </c>
     </row>
-    <row r="156" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A156">
         <v>1997</v>
       </c>
@@ -22439,7 +22436,7 @@
         <v>0.10390976252948939</v>
       </c>
     </row>
-    <row r="157" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A157">
         <v>1997</v>
       </c>
@@ -22579,7 +22576,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A158">
         <v>1998</v>
       </c>
@@ -22719,7 +22716,7 @@
         <v>0.15998743541205107</v>
       </c>
     </row>
-    <row r="159" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A159">
         <v>1998</v>
       </c>
@@ -22859,7 +22856,7 @@
         <v>0.10457608095970851</v>
       </c>
     </row>
-    <row r="160" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A160">
         <v>1998</v>
       </c>
@@ -22999,7 +22996,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A161">
         <v>1998</v>
       </c>
@@ -23139,7 +23136,7 @@
         <v>4.8927873045533567E-2</v>
       </c>
     </row>
-    <row r="162" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A162">
         <v>1998</v>
       </c>
@@ -23279,7 +23276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A163">
         <v>1998</v>
       </c>
@@ -23419,7 +23416,7 @@
         <v>5.2048890308667252E-2</v>
       </c>
     </row>
-    <row r="164" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A164">
         <v>1998</v>
       </c>
@@ -23559,7 +23556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A165">
         <v>1998</v>
       </c>
@@ -23699,7 +23696,7 @@
         <v>5.4756290656475984E-2</v>
       </c>
     </row>
-    <row r="166" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A166">
         <v>1998</v>
       </c>
@@ -23839,7 +23836,7 @@
         <v>0.15705178724699081</v>
       </c>
     </row>
-    <row r="167" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A167">
         <v>1998</v>
       </c>
@@ -23979,7 +23976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A168">
         <v>1998</v>
       </c>
@@ -24119,7 +24116,7 @@
         <v>5.658946718488421E-2</v>
       </c>
     </row>
-    <row r="169" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A169">
         <v>1998</v>
       </c>
@@ -24259,7 +24256,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A170">
         <v>1999</v>
       </c>
@@ -24399,7 +24396,7 @@
         <v>5.6508663088776348E-2</v>
       </c>
     </row>
-    <row r="171" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A171">
         <v>1999</v>
       </c>
@@ -24539,7 +24536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A172">
         <v>1999</v>
       </c>
@@ -24679,7 +24676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A173">
         <v>1999</v>
       </c>
@@ -24819,7 +24816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A174">
         <v>1999</v>
       </c>
@@ -24959,7 +24956,7 @@
         <v>9.6452306992936845E-2</v>
       </c>
     </row>
-    <row r="175" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A175">
         <v>1999</v>
       </c>
@@ -25099,7 +25096,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A176">
         <v>1999</v>
       </c>
@@ -25239,7 +25236,7 @@
         <v>5.5431628114239302E-2</v>
       </c>
     </row>
-    <row r="177" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A177">
         <v>1999</v>
       </c>
@@ -25379,7 +25376,7 @@
         <v>0.23701354219259319</v>
       </c>
     </row>
-    <row r="178" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A178">
         <v>1999</v>
       </c>
@@ -25519,7 +25516,7 @@
         <v>0.1077867461413872</v>
       </c>
     </row>
-    <row r="179" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A179">
         <v>1999</v>
       </c>
@@ -25659,7 +25656,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A180">
         <v>1999</v>
       </c>
@@ -25799,7 +25796,7 @@
         <v>5.2842731061189072E-2</v>
       </c>
     </row>
-    <row r="181" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A181">
         <v>1999</v>
       </c>
@@ -25939,7 +25936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A182">
         <v>2000</v>
       </c>
@@ -26079,7 +26076,7 @@
         <v>5.8544122343726579E-2</v>
       </c>
     </row>
-    <row r="183" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A183">
         <v>2000</v>
       </c>
@@ -26219,7 +26216,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A184">
         <v>2000</v>
       </c>
@@ -26359,7 +26356,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A185">
         <v>2000</v>
       </c>
@@ -26499,7 +26496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A186">
         <v>2000</v>
       </c>
@@ -26639,7 +26636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A187">
         <v>2000</v>
       </c>
@@ -26779,7 +26776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A188">
         <v>2000</v>
       </c>
@@ -26919,7 +26916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A189">
         <v>2000</v>
       </c>
@@ -27059,7 +27056,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="190" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A190">
         <v>2000</v>
       </c>
@@ -27199,7 +27196,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A191">
         <v>2000</v>
       </c>
@@ -27339,7 +27336,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="192" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A192">
         <v>2000</v>
       </c>
@@ -27479,7 +27476,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A193">
         <v>2000</v>
       </c>
@@ -27619,7 +27616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="194" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A194">
         <v>2001</v>
       </c>
@@ -27759,7 +27756,7 @@
         <v>0.16555175270678665</v>
       </c>
     </row>
-    <row r="195" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A195">
         <v>2001</v>
       </c>
@@ -27899,7 +27896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A196">
         <v>2001</v>
       </c>
@@ -28039,7 +28036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A197">
         <v>2001</v>
       </c>
@@ -28179,7 +28176,7 @@
         <v>5.2742593265274196E-2</v>
       </c>
     </row>
-    <row r="198" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A198">
         <v>2001</v>
       </c>
@@ -28319,7 +28316,7 @@
         <v>0.10831734953416297</v>
       </c>
     </row>
-    <row r="199" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A199">
         <v>2001</v>
       </c>
@@ -28459,7 +28456,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="200" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A200">
         <v>2001</v>
       </c>
@@ -28599,7 +28596,7 @@
         <v>5.6218510010380585E-2</v>
       </c>
     </row>
-    <row r="201" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A201">
         <v>2001</v>
       </c>
@@ -28739,7 +28736,7 @@
         <v>0.11125182042878982</v>
       </c>
     </row>
-    <row r="202" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A202">
         <v>2001</v>
       </c>
@@ -28879,7 +28876,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="203" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A203">
         <v>2001</v>
       </c>
@@ -29019,7 +29016,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="204" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A204">
         <v>2001</v>
       </c>
@@ -29159,7 +29156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="205" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A205">
         <v>2001</v>
       </c>
@@ -29299,7 +29296,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="206" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A206">
         <v>2002</v>
       </c>
@@ -29439,7 +29436,7 @@
         <v>0.11839619943918275</v>
       </c>
     </row>
-    <row r="207" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A207">
         <v>2002</v>
       </c>
@@ -29579,7 +29576,7 @@
         <v>5.8190093386647851E-2</v>
       </c>
     </row>
-    <row r="208" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A208">
         <v>2002</v>
       </c>
@@ -29719,7 +29716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="209" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A209">
         <v>2002</v>
       </c>
@@ -29859,7 +29856,7 @@
         <v>5.7228588310741631E-2</v>
       </c>
     </row>
-    <row r="210" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A210">
         <v>2002</v>
       </c>
@@ -29999,7 +29996,7 @@
         <v>0.1074798432263461</v>
       </c>
     </row>
-    <row r="211" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A211">
         <v>2002</v>
       </c>
@@ -30139,7 +30136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="212" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A212">
         <v>2002</v>
       </c>
@@ -30279,7 +30276,7 @@
         <v>6.5636627546703546E-2</v>
       </c>
     </row>
-    <row r="213" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A213">
         <v>2002</v>
       </c>
@@ -30419,7 +30416,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="214" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A214">
         <v>2002</v>
       </c>
@@ -30559,7 +30556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="215" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A215">
         <v>2002</v>
       </c>
@@ -30699,7 +30696,7 @@
         <v>5.3692820942849433E-2</v>
       </c>
     </row>
-    <row r="216" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A216">
         <v>2002</v>
       </c>
@@ -30839,7 +30836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="217" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A217">
         <v>2002</v>
       </c>
@@ -30979,7 +30976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="218" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A218">
         <v>2003</v>
       </c>
@@ -31119,7 +31116,7 @@
         <v>5.4987865599311708E-2</v>
       </c>
     </row>
-    <row r="219" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A219">
         <v>2003</v>
       </c>
@@ -31259,7 +31256,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="220" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A220">
         <v>2003</v>
       </c>
@@ -31399,7 +31396,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="221" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A221">
         <v>2003</v>
       </c>
@@ -31539,7 +31536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="222" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A222">
         <v>2003</v>
       </c>
@@ -31679,7 +31676,7 @@
         <v>0.16009350904484385</v>
       </c>
     </row>
-    <row r="223" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A223">
         <v>2003</v>
       </c>
@@ -31819,7 +31816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="224" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A224">
         <v>2003</v>
       </c>
@@ -31959,7 +31956,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="225" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A225">
         <v>2003</v>
       </c>
@@ -32099,7 +32096,7 @@
         <v>5.3988080505931048E-2</v>
       </c>
     </row>
-    <row r="226" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A226">
         <v>2003</v>
       </c>
@@ -32239,7 +32236,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="227" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A227">
         <v>2003</v>
       </c>
@@ -32379,7 +32376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="228" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A228">
         <v>2003</v>
       </c>
@@ -32519,7 +32516,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A229">
         <v>2003</v>
       </c>
@@ -32659,7 +32656,7 @@
         <v>0.31806901992420428</v>
       </c>
     </row>
-    <row r="230" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A230">
         <v>2004</v>
       </c>
@@ -32799,7 +32796,7 @@
         <v>0.15859041243885005</v>
       </c>
     </row>
-    <row r="231" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A231">
         <v>2004</v>
       </c>
@@ -32939,7 +32936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="232" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A232">
         <v>2004</v>
       </c>
@@ -33079,7 +33076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="233" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A233">
         <v>2004</v>
       </c>
@@ -33219,7 +33216,7 @@
         <v>5.1535172359124061E-2</v>
       </c>
     </row>
-    <row r="234" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A234">
         <v>2004</v>
       </c>
@@ -33359,7 +33356,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="235" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A235">
         <v>2004</v>
       </c>
@@ -33499,7 +33496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="236" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A236">
         <v>2004</v>
       </c>
@@ -33639,7 +33636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="237" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A237">
         <v>2004</v>
       </c>
@@ -33779,7 +33776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="238" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A238">
         <v>2004</v>
       </c>
@@ -33919,7 +33916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="239" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A239">
         <v>2004</v>
       </c>
@@ -34059,7 +34056,7 @@
         <v>4.9892839511491094E-2</v>
       </c>
     </row>
-    <row r="240" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A240">
         <v>2004</v>
       </c>
@@ -34199,7 +34196,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="241" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A241">
         <v>2004</v>
       </c>
@@ -34339,7 +34336,7 @@
         <v>0.10307722380667021</v>
       </c>
     </row>
-    <row r="242" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A242">
         <v>2005</v>
       </c>
@@ -34479,7 +34476,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="243" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A243">
         <v>2005</v>
       </c>
@@ -34619,7 +34616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="244" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A244">
         <v>2005</v>
       </c>
@@ -34759,7 +34756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="245" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A245">
         <v>2005</v>
       </c>
@@ -34899,7 +34896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="246" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A246">
         <v>2005</v>
       </c>
@@ -35039,7 +35036,7 @@
         <v>5.1203411799097209E-2</v>
       </c>
     </row>
-    <row r="247" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A247">
         <v>2005</v>
       </c>
@@ -35179,7 +35176,7 @@
         <v>0.10452405214309693</v>
       </c>
     </row>
-    <row r="248" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A248">
         <v>2005</v>
       </c>
@@ -35319,7 +35316,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="249" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A249">
         <v>2005</v>
       </c>
@@ -35459,7 +35456,7 @@
         <v>0.1141746495649268</v>
       </c>
     </row>
-    <row r="250" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A250">
         <v>2005</v>
       </c>
@@ -35599,7 +35596,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="251" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A251">
         <v>2005</v>
       </c>
@@ -35739,7 +35736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="252" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A252">
         <v>2005</v>
       </c>
@@ -35879,7 +35876,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="253" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A253">
         <v>2005</v>
       </c>
@@ -36019,7 +36016,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="254" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A254">
         <v>2006</v>
       </c>
@@ -36159,7 +36156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="255" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A255">
         <v>2006</v>
       </c>
@@ -36299,7 +36296,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="256" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A256">
         <v>2006</v>
       </c>
@@ -36439,7 +36436,7 @@
         <v>4.6525101742501983E-2</v>
       </c>
     </row>
-    <row r="257" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A257">
         <v>2006</v>
       </c>
@@ -36579,7 +36576,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="258" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A258">
         <v>2006</v>
       </c>
@@ -36719,7 +36716,7 @@
         <v>5.2732547600112277E-2</v>
       </c>
     </row>
-    <row r="259" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A259">
         <v>2006</v>
       </c>
@@ -36859,7 +36856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="260" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A260">
         <v>2006</v>
       </c>
@@ -36999,7 +36996,7 @@
         <v>5.7622490283505468E-2</v>
       </c>
     </row>
-    <row r="261" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A261">
         <v>2006</v>
       </c>
@@ -37139,7 +37136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="262" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A262">
         <v>2006</v>
       </c>
@@ -37279,7 +37276,7 @@
         <v>9.8575626100812636E-2</v>
       </c>
     </row>
-    <row r="263" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A263">
         <v>2006</v>
       </c>
@@ -37419,7 +37416,7 @@
         <v>4.7985492768834848E-2</v>
       </c>
     </row>
-    <row r="264" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A264">
         <v>2006</v>
       </c>
@@ -37559,7 +37556,7 @@
         <v>4.3783322138046102E-2</v>
       </c>
     </row>
-    <row r="265" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A265">
         <v>2006</v>
       </c>
@@ -37699,7 +37696,7 @@
         <v>4.7026141532598306E-2</v>
       </c>
     </row>
-    <row r="266" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A266">
         <v>2007</v>
       </c>
@@ -37839,7 +37836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="267" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A267">
         <v>2007</v>
       </c>
@@ -37979,7 +37976,7 @@
         <v>5.0807164510091152E-2</v>
       </c>
     </row>
-    <row r="268" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A268">
         <v>2007</v>
       </c>
@@ -38119,7 +38116,7 @@
         <v>4.5967984957745553E-2</v>
       </c>
     </row>
-    <row r="269" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A269">
         <v>2007</v>
       </c>
@@ -38259,7 +38256,7 @@
         <v>4.5068763769589938E-2</v>
       </c>
     </row>
-    <row r="270" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A270">
         <v>2007</v>
       </c>
@@ -38399,7 +38396,7 @@
         <v>4.5569652981228302E-2</v>
       </c>
     </row>
-    <row r="271" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A271">
         <v>2007</v>
       </c>
@@ -38539,7 +38536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="272" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A272">
         <v>2007</v>
       </c>
@@ -38679,7 +38676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="273" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A273">
         <v>2007</v>
       </c>
@@ -38819,7 +38816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="274" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A274">
         <v>2007</v>
       </c>
@@ -38959,7 +38956,7 @@
         <v>5.0047105480088547E-2</v>
       </c>
     </row>
-    <row r="275" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A275">
         <v>2007</v>
       </c>
@@ -39099,7 +39096,7 @@
         <v>9.7629833630737822E-2</v>
       </c>
     </row>
-    <row r="276" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A276">
         <v>2007</v>
       </c>
@@ -39239,7 +39236,7 @@
         <v>4.7991707768664529E-2</v>
       </c>
     </row>
-    <row r="277" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A277">
         <v>2007</v>
       </c>
@@ -39379,7 +39376,7 @@
         <v>5.1430353029506409E-2</v>
       </c>
     </row>
-    <row r="278" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A278">
         <v>2008</v>
       </c>
@@ -39519,7 +39516,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="279" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A279">
         <v>2008</v>
       </c>
@@ -39659,7 +39656,7 @@
         <v>0.20586752840046235</v>
       </c>
     </row>
-    <row r="280" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A280">
         <v>2008</v>
       </c>
@@ -39799,7 +39796,7 @@
         <v>4.7432765929270815E-2</v>
       </c>
     </row>
-    <row r="281" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A281">
         <v>2008</v>
       </c>
@@ -39939,7 +39936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="282" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A282">
         <v>2008</v>
       </c>
@@ -40079,7 +40076,7 @@
         <v>0.14232133564196134</v>
       </c>
     </row>
-    <row r="283" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A283">
         <v>2008</v>
       </c>
@@ -40219,7 +40216,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="284" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A284">
         <v>2008</v>
       </c>
@@ -40359,7 +40356,7 @@
         <v>0.1127060475975576</v>
       </c>
     </row>
-    <row r="285" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A285">
         <v>2008</v>
       </c>
@@ -40499,7 +40496,7 @@
         <v>9.1532825553504227E-2</v>
       </c>
     </row>
-    <row r="286" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A286">
         <v>2008</v>
       </c>
@@ -40639,7 +40636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="287" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A287">
         <v>2008</v>
       </c>
@@ -40779,7 +40776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="288" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A288">
         <v>2008</v>
       </c>
@@ -40919,7 +40916,7 @@
         <v>0.12023021510389985</v>
       </c>
     </row>
-    <row r="289" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A289">
         <v>2008</v>
       </c>
@@ -41059,7 +41056,7 @@
         <v>5.939089508363659E-2</v>
       </c>
     </row>
-    <row r="290" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A290">
         <v>2009</v>
       </c>
@@ -41199,7 +41196,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="291" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A291">
         <v>2009</v>
       </c>
@@ -41339,7 +41336,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="292" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A292">
         <v>2009</v>
       </c>
@@ -41479,7 +41476,7 @@
         <v>5.9858835015858411E-2</v>
       </c>
     </row>
-    <row r="293" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A293">
         <v>2009</v>
       </c>
@@ -41619,7 +41616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="294" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A294">
         <v>2009</v>
       </c>
@@ -41759,7 +41756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="295" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A295">
         <v>2009</v>
       </c>
@@ -41899,7 +41896,7 @@
         <v>6.4877004208772085E-2</v>
       </c>
     </row>
-    <row r="296" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A296">
         <v>2009</v>
       </c>
@@ -42039,7 +42036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="297" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A297">
         <v>2009</v>
       </c>
@@ -42179,7 +42176,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="298" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A298">
         <v>2009</v>
       </c>
@@ -42319,7 +42316,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="299" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A299">
         <v>2009</v>
       </c>
@@ -42459,7 +42456,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="300" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A300">
         <v>2009</v>
       </c>
@@ -42599,7 +42596,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="301" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A301">
         <v>2009</v>
       </c>
@@ -42739,7 +42736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="302" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A302">
         <v>2010</v>
       </c>
@@ -42879,7 +42876,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="303" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A303">
         <v>2010</v>
       </c>
@@ -43019,7 +43016,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="304" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A304">
         <v>2010</v>
       </c>
@@ -43159,7 +43156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="305" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A305">
         <v>2010</v>
       </c>
@@ -43299,7 +43296,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="306" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A306">
         <v>2010</v>
       </c>
@@ -43439,7 +43436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="307" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A307">
         <v>2010</v>
       </c>
@@ -43579,7 +43576,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="308" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A308">
         <v>2010</v>
       </c>
@@ -43719,7 +43716,7 @@
         <v>5.7972342879683877E-2</v>
       </c>
     </row>
-    <row r="309" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A309">
         <v>2010</v>
       </c>
@@ -43859,7 +43856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="310" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A310">
         <v>2010</v>
       </c>
@@ -43999,7 +43996,7 @@
         <v>0.10392344033970213</v>
       </c>
     </row>
-    <row r="311" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A311">
         <v>2010</v>
       </c>
@@ -44139,7 +44136,7 @@
         <v>4.9624012093502298E-2</v>
       </c>
     </row>
-    <row r="312" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A312">
         <v>2010</v>
       </c>
@@ -44279,7 +44276,7 @@
         <v>5.686995040538699E-2</v>
       </c>
     </row>
-    <row r="313" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A313">
         <v>2010</v>
       </c>
@@ -44419,7 +44416,7 @@
         <v>5.4879685784128392E-2</v>
       </c>
     </row>
-    <row r="314" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A314">
         <v>2011</v>
       </c>
@@ -44559,7 +44556,7 @@
         <v>0.11452798994760664</v>
       </c>
     </row>
-    <row r="315" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A315">
         <v>2011</v>
       </c>
@@ -44699,7 +44696,7 @@
         <v>5.4558506718388314E-2</v>
       </c>
     </row>
-    <row r="316" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A316">
         <v>2011</v>
       </c>
@@ -44839,7 +44836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="317" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A317">
         <v>2011</v>
       </c>
@@ -44979,7 +44976,7 @@
         <v>5.5414990836561324E-2</v>
       </c>
     </row>
-    <row r="318" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A318">
         <v>2011</v>
       </c>
@@ -45119,7 +45116,7 @@
         <v>5.9417941180833309E-2</v>
       </c>
     </row>
-    <row r="319" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A319">
         <v>2011</v>
       </c>
@@ -45259,7 +45256,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="320" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A320">
         <v>2011</v>
       </c>
@@ -45399,7 +45396,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="321" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A321">
         <v>2011</v>
       </c>
@@ -45539,7 +45536,7 @@
         <v>0.22798166739360223</v>
       </c>
     </row>
-    <row r="322" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A322">
         <v>2011</v>
       </c>
@@ -45679,7 +45676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="323" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A323">
         <v>2011</v>
       </c>
@@ -45819,7 +45816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="324" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A324">
         <v>2011</v>
       </c>
@@ -45959,7 +45956,7 @@
         <v>6.0564160346984863E-2</v>
       </c>
     </row>
-    <row r="325" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A325">
         <v>2011</v>
       </c>
@@ -46099,7 +46096,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="326" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A326">
         <v>2012</v>
       </c>
@@ -46239,7 +46236,7 @@
         <v>6.043768192523092E-2</v>
       </c>
     </row>
-    <row r="327" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A327">
         <v>2012</v>
       </c>
@@ -46379,7 +46376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="328" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A328">
         <v>2012</v>
       </c>
@@ -46519,7 +46516,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="329" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A329">
         <v>2012</v>
       </c>
@@ -46659,7 +46656,7 @@
         <v>0.11766587911437754</v>
       </c>
     </row>
-    <row r="330" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A330">
         <v>2012</v>
       </c>
@@ -46799,7 +46796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="331" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A331">
         <v>2012</v>
       </c>
@@ -46939,7 +46936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="332" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A332">
         <v>2012</v>
       </c>
@@ -47079,7 +47076,7 @@
         <v>7.351121515365544E-2</v>
       </c>
     </row>
-    <row r="333" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A333">
         <v>2012</v>
       </c>
@@ -47219,7 +47216,7 @@
         <v>0.12352876060514201</v>
       </c>
     </row>
-    <row r="334" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A334">
         <v>2012</v>
       </c>
@@ -47359,7 +47356,7 @@
         <v>6.1028603351477424E-2</v>
       </c>
     </row>
-    <row r="335" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A335">
         <v>2012</v>
       </c>
@@ -47499,7 +47496,7 @@
         <v>0.22379858976875255</v>
       </c>
     </row>
-    <row r="336" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A336">
         <v>2012</v>
       </c>
@@ -47639,7 +47636,7 @@
         <v>5.4411811159368148E-2</v>
       </c>
     </row>
-    <row r="337" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A337">
         <v>2012</v>
       </c>
@@ -47779,7 +47776,7 @@
         <v>0.10198109469309774</v>
       </c>
     </row>
-    <row r="338" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A338">
         <v>2013</v>
       </c>
@@ -47919,7 +47916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="339" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A339">
         <v>2013</v>
       </c>
@@ -48059,7 +48056,7 @@
         <v>3.9308759901258684E-2</v>
       </c>
     </row>
-    <row r="340" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A340">
         <v>2013</v>
       </c>
@@ -48199,7 +48196,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="341" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A341">
         <v>2013</v>
       </c>
@@ -48339,7 +48336,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="342" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A342">
         <v>2013</v>
       </c>
@@ -48479,7 +48476,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="343" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A343">
         <v>2013</v>
       </c>
@@ -48619,7 +48616,7 @@
         <v>4.8809415343179868E-2</v>
       </c>
     </row>
-    <row r="344" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A344">
         <v>2013</v>
       </c>
@@ -48759,7 +48756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="345" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A345">
         <v>2013</v>
       </c>
@@ -48899,7 +48896,7 @@
         <v>5.1557405178363512E-2</v>
       </c>
     </row>
-    <row r="346" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A346">
         <v>2013</v>
       </c>
@@ -49039,7 +49036,7 @@
         <v>5.7157294429949858E-2</v>
       </c>
     </row>
-    <row r="347" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A347">
         <v>2013</v>
       </c>
@@ -49179,7 +49176,7 @@
         <v>5.5744525364467078E-2</v>
       </c>
     </row>
-    <row r="348" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A348">
         <v>2013</v>
       </c>
@@ -49319,7 +49316,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="349" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A349">
         <v>2013</v>
       </c>
@@ -49459,7 +49456,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="350" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A350">
         <v>2014</v>
       </c>
@@ -49599,7 +49596,7 @@
         <v>5.7144897260915921E-2</v>
       </c>
     </row>
-    <row r="351" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A351">
         <v>2014</v>
       </c>
@@ -49739,7 +49736,7 @@
         <v>5.3292169483429797E-2</v>
       </c>
     </row>
-    <row r="352" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A352">
         <v>2014</v>
       </c>
@@ -49879,7 +49876,7 @@
         <v>0.17866801093606388</v>
       </c>
     </row>
-    <row r="353" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A353">
         <v>2014</v>
       </c>
@@ -50019,7 +50016,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="354" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A354">
         <v>2014</v>
       </c>
@@ -50159,7 +50156,7 @@
         <v>5.8477523479055854E-2</v>
       </c>
     </row>
-    <row r="355" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A355">
         <v>2014</v>
       </c>
@@ -50299,7 +50296,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="356" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A356">
         <v>2014</v>
       </c>
@@ -50439,7 +50436,7 @@
         <v>5.9556726681984078E-2</v>
       </c>
     </row>
-    <row r="357" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A357">
         <v>2014</v>
       </c>
@@ -50579,7 +50576,7 @@
         <v>5.5608080339062123E-2</v>
       </c>
     </row>
-    <row r="358" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A358">
         <v>2014</v>
       </c>
@@ -50719,7 +50716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="359" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A359">
         <v>2014</v>
       </c>
@@ -50859,7 +50856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="360" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A360">
         <v>2014</v>
       </c>
@@ -50999,7 +50996,7 @@
         <v>6.4328524801466197E-2</v>
       </c>
     </row>
-    <row r="361" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A361">
         <v>2014</v>
       </c>
@@ -51139,7 +51136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="362" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A362">
         <v>2015</v>
       </c>
@@ -51279,7 +51276,7 @@
         <v>0.13527708191802537</v>
       </c>
     </row>
-    <row r="363" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A363">
         <v>2015</v>
       </c>
@@ -51419,7 +51416,7 @@
         <v>0.30465798976617459</v>
       </c>
     </row>
-    <row r="364" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A364">
         <v>2015</v>
       </c>
@@ -51559,7 +51556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="365" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A365">
         <v>2015</v>
       </c>
@@ -51699,7 +51696,7 @@
         <v>6.7943550611325829E-2</v>
       </c>
     </row>
-    <row r="366" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A366">
         <v>2015</v>
       </c>
@@ -51839,7 +51836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="367" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A367">
         <v>2015</v>
       </c>
@@ -51979,7 +51976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="368" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A368">
         <v>2015</v>
       </c>
@@ -52119,7 +52116,7 @@
         <v>0.14284806622716481</v>
       </c>
     </row>
-    <row r="369" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A369">
         <v>2015</v>
       </c>
@@ -52259,7 +52256,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="370" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A370">
         <v>2015</v>
       </c>
@@ -52399,7 +52396,7 @@
         <v>0.14663554794356803</v>
       </c>
     </row>
-    <row r="371" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A371">
         <v>2015</v>
       </c>
@@ -52539,7 +52536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="372" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A372">
         <v>2015</v>
       </c>
@@ -52679,7 +52676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="373" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A373">
         <v>2015</v>
       </c>
@@ -52819,7 +52816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="374" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A374">
         <v>2016</v>
       </c>
@@ -52959,7 +52956,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="375" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A375">
         <v>2016</v>
       </c>
@@ -53099,7 +53096,7 @@
         <v>0.20386602057785286</v>
       </c>
     </row>
-    <row r="376" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A376">
         <v>2016</v>
       </c>
@@ -53239,7 +53236,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="377" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A377">
         <v>2016</v>
       </c>
@@ -53379,7 +53376,7 @@
         <v>0.1461130603329166</v>
       </c>
     </row>
-    <row r="378" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A378">
         <v>2016</v>
       </c>
@@ -53519,7 +53516,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="379" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A379">
         <v>2016</v>
       </c>
@@ -53659,7 +53656,7 @@
         <v>9.5896575564429876E-2</v>
       </c>
     </row>
-    <row r="380" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A380">
         <v>2016</v>
       </c>
@@ -53799,7 +53796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="381" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A381">
         <v>2016</v>
       </c>
@@ -53939,7 +53936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="382" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A382">
         <v>2016</v>
       </c>
@@ -54079,7 +54076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="383" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A383">
         <v>2016</v>
       </c>
@@ -54219,7 +54216,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="384" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A384">
         <v>2016</v>
       </c>
@@ -54359,7 +54356,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="385" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A385">
         <v>2016</v>
       </c>
@@ -54499,7 +54496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="386" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A386">
         <v>2017</v>
       </c>
@@ -54639,7 +54636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="387" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A387">
         <v>2017</v>
       </c>
@@ -54779,7 +54776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="388" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A388">
         <v>2017</v>
       </c>
@@ -54919,7 +54916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="389" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A389">
         <v>2017</v>
       </c>
@@ -55059,7 +55056,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="390" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A390">
         <v>2017</v>
       </c>
@@ -55199,7 +55196,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="391" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A391">
         <v>2017</v>
       </c>
@@ -55339,7 +55336,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="392" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A392">
         <v>2017</v>
       </c>
@@ -55479,7 +55476,7 @@
         <v>0.11039887941800632</v>
       </c>
     </row>
-    <row r="393" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A393">
         <v>2017</v>
       </c>
@@ -55619,7 +55616,7 @@
         <v>0.11794042935336593</v>
       </c>
     </row>
-    <row r="394" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A394">
         <v>2017</v>
       </c>
@@ -55759,7 +55756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="395" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A395">
         <v>2017</v>
       </c>
@@ -55899,7 +55896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="396" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A396">
         <v>2017</v>
       </c>
@@ -56039,7 +56036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="397" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A397">
         <v>2017</v>
       </c>
@@ -56179,7 +56176,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="398" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A398">
         <v>2018</v>
       </c>
@@ -56319,7 +56316,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="399" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A399">
         <v>2018</v>
       </c>
@@ -56459,7 +56456,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="400" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A400">
         <v>2018</v>
       </c>
@@ -56599,7 +56596,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="401" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A401">
         <v>2018</v>
       </c>
@@ -56739,7 +56736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="402" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A402">
         <v>2018</v>
       </c>
@@ -56879,7 +56876,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="403" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A403">
         <v>2018</v>
       </c>
@@ -57019,7 +57016,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="404" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A404">
         <v>2018</v>
       </c>
@@ -57159,7 +57156,7 @@
         <v>0.11753958407963547</v>
       </c>
     </row>
-    <row r="405" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A405">
         <v>2018</v>
       </c>
@@ -57299,7 +57296,7 @@
         <v>0.11266521941450305</v>
       </c>
     </row>
-    <row r="406" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A406">
         <v>2018</v>
       </c>
@@ -57439,7 +57436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="407" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A407">
         <v>2018</v>
       </c>
@@ -57579,7 +57576,7 @@
         <v>0.23772659301757812</v>
       </c>
     </row>
-    <row r="408" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A408">
         <v>2018</v>
       </c>
@@ -57719,7 +57716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="409" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A409">
         <v>2018</v>
       </c>
@@ -57859,7 +57856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="410" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A410">
         <v>2019</v>
       </c>
@@ -57999,7 +57996,7 @@
         <v>0.59153895990393968</v>
       </c>
     </row>
-    <row r="411" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A411">
         <v>2019</v>
       </c>
@@ -58139,7 +58136,7 @@
         <v>0.12540431488725476</v>
       </c>
     </row>
-    <row r="412" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A412">
         <v>2019</v>
       </c>
@@ -58279,7 +58276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="413" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A413">
         <v>2019</v>
       </c>
@@ -58419,7 +58416,7 @@
         <v>0.15542810613458807</v>
       </c>
     </row>
-    <row r="414" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A414">
         <v>2019</v>
       </c>
@@ -58559,7 +58556,7 @@
         <v>0.25195644747826362</v>
       </c>
     </row>
-    <row r="415" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A415">
         <v>2019</v>
       </c>
@@ -58699,7 +58696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="416" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A416">
         <v>2019</v>
       </c>
@@ -58839,7 +58836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="417" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A417">
         <v>2019</v>
       </c>
@@ -58979,7 +58976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="418" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A418">
         <v>2019</v>
       </c>
@@ -59119,7 +59116,7 @@
         <v>0.14633627195616025</v>
       </c>
     </row>
-    <row r="419" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A419">
         <v>2019</v>
       </c>
@@ -59259,7 +59256,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="420" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A420">
         <v>2019</v>
       </c>
@@ -59399,7 +59396,7 @@
         <v>0.15001831054687501</v>
       </c>
     </row>
-    <row r="421" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A421">
         <v>2019</v>
       </c>
@@ -59539,7 +59536,7 @@
         <v>0.31482741411994486</v>
       </c>
     </row>
-    <row r="422" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A422">
         <v>2020</v>
       </c>
@@ -59679,7 +59676,7 @@
         <v>0.13185242244175502</v>
       </c>
     </row>
-    <row r="423" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A423">
         <v>2020</v>
       </c>
@@ -59819,7 +59816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="424" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A424">
         <v>2020</v>
       </c>
@@ -59959,7 +59956,7 @@
         <v>0.32746134124677007</v>
       </c>
     </row>
-    <row r="425" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A425">
         <v>2020</v>
       </c>
@@ -60099,7 +60096,7 @@
         <v>0.1757860271208877</v>
       </c>
     </row>
-    <row r="426" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A426">
         <v>2020</v>
       </c>
@@ -60239,10 +60236,8 @@
         <v>0.21106313523792083</v>
       </c>
     </row>
-    <row r="427" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A427" s="1" t="s">
-        <v>45</v>
-      </c>
+    <row r="427" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="A427" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>